<commit_message>
Changes In the format
Smooth table which is editable in whole
</commit_message>
<xml_diff>
--- a/external_data_2.xlsx
+++ b/external_data_2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,16 +514,30 @@
           <t>kat</t>
         </is>
       </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Silt (%)</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Kami</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="D2" t="n">
         <v>1</v>
@@ -560,16 +574,26 @@
       </c>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" t="n">
-        <v>3</v>
-      </c>
-      <c r="C3" t="n">
-        <v>10</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="D3" t="n">
         <v>70</v>
@@ -610,13 +634,17 @@
       <c r="P3" t="n">
         <v>5</v>
       </c>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="n">
-        <v>3</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -658,13 +686,17 @@
       </c>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>5</v>
       </c>
-      <c r="B5" t="n">
-        <v>5</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -710,13 +742,17 @@
       <c r="P5" t="n">
         <v>40</v>
       </c>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>5</v>
       </c>
-      <c r="B6" t="n">
-        <v>5</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -762,13 +798,17 @@
       <c r="P6" t="n">
         <v>40</v>
       </c>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="n">
-        <v>5</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -814,13 +854,17 @@
       <c r="P7" t="n">
         <v>40</v>
       </c>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>5</v>
       </c>
-      <c r="B8" t="n">
-        <v>5</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -866,6 +910,8 @@
       <c r="P8" t="n">
         <v>40</v>
       </c>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -920,6 +966,8 @@
       <c r="P9" t="n">
         <v>2</v>
       </c>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -974,6 +1022,8 @@
       <c r="P10" t="n">
         <v>2</v>
       </c>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1028,6 +1078,8 @@
       <c r="P11" t="n">
         <v>2</v>
       </c>
+      <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1082,6 +1134,8 @@
       <c r="P12" t="n">
         <v>2</v>
       </c>
+      <c r="Q12" t="inlineStr"/>
+      <c r="R12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1136,6 +1190,8 @@
       <c r="P13" t="n">
         <v>2</v>
       </c>
+      <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1190,6 +1246,8 @@
       <c r="P14" t="n">
         <v>2</v>
       </c>
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1244,12 +1302,12 @@
       <c r="P15" t="n">
         <v>5</v>
       </c>
+      <c r="Q15" t="inlineStr"/>
+      <c r="R15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A16" t="n">
+        <v>7</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1267,61 +1325,679 @@
       <c r="E16" t="n">
         <v>0</v>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="F16" t="n">
+        <v>5</v>
+      </c>
+      <c r="G16" t="n">
+        <v>5</v>
+      </c>
+      <c r="H16" t="n">
+        <v>5</v>
+      </c>
+      <c r="I16" t="n">
+        <v>5</v>
+      </c>
+      <c r="J16" t="n">
+        <v>5</v>
+      </c>
+      <c r="K16" t="n">
+        <v>5</v>
+      </c>
+      <c r="L16" t="n">
+        <v>5</v>
+      </c>
+      <c r="M16" t="n">
+        <v>5</v>
+      </c>
+      <c r="N16" t="n">
+        <v>5</v>
+      </c>
+      <c r="O16" t="n">
+        <v>5</v>
+      </c>
+      <c r="P16" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q16" t="inlineStr"/>
+      <c r="R16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>2</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="n">
+        <v>70</v>
+      </c>
+      <c r="E17" t="n">
+        <v>55</v>
+      </c>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>2</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="D18" t="n">
+        <v>55</v>
+      </c>
+      <c r="E18" t="n">
+        <v>55</v>
+      </c>
+      <c r="F18" t="n">
+        <v>7</v>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="n">
+        <v>7</v>
+      </c>
+      <c r="I18" t="n">
+        <v>7</v>
+      </c>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="n">
+        <v>7</v>
+      </c>
+      <c r="R18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>2</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>30-40</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>60</v>
+      </c>
+      <c r="E19" t="n">
+        <v>60</v>
+      </c>
+      <c r="F19" t="n">
+        <v>70</v>
+      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="n">
+        <v>50</v>
+      </c>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="n">
+        <v>30</v>
+      </c>
+      <c r="R19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="K20" t="n">
+        <v>1</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
+      <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>2</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>70</v>
+      </c>
+      <c r="E21" t="n">
+        <v>18</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="K21" t="n">
+        <v>1</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="O21" t="n">
+        <v>2</v>
+      </c>
+      <c r="P21" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>3</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>10-20</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>80</v>
+      </c>
+      <c r="E22" t="n">
+        <v>25</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="K22" t="n">
+        <v>1</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr"/>
+      <c r="R22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>5</v>
+      </c>
+      <c r="B23" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>10-20</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>29</v>
+      </c>
+      <c r="E23" t="n">
+        <v>80</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="K23" t="n">
+        <v>1</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="O23" t="n">
+        <v>30</v>
+      </c>
+      <c r="P23" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q23" t="inlineStr"/>
+      <c r="R23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>5</v>
+      </c>
+      <c r="B24" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>20-40</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>29</v>
+      </c>
+      <c r="E24" t="n">
+        <v>80</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="K24" t="n">
+        <v>1</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="O24" t="n">
+        <v>30</v>
+      </c>
+      <c r="P24" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q24" t="inlineStr"/>
+      <c r="R24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>5</v>
+      </c>
+      <c r="B25" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>40-60</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>29</v>
+      </c>
+      <c r="E25" t="n">
+        <v>80</v>
+      </c>
+      <c r="F25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="K25" t="n">
+        <v>1</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="O25" t="n">
+        <v>30</v>
+      </c>
+      <c r="P25" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q25" t="inlineStr"/>
+      <c r="R25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>5</v>
+      </c>
+      <c r="B26" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="N16" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="P16" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>60-90</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>29</v>
+      </c>
+      <c r="E26" t="n">
+        <v>80</v>
+      </c>
+      <c r="F26" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1</v>
+      </c>
+      <c r="H26" t="n">
+        <v>1</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="K26" t="n">
+        <v>1</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="O26" t="n">
+        <v>30</v>
+      </c>
+      <c r="P26" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q26" t="inlineStr"/>
+      <c r="R26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>1</v>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="n">
+        <v>55</v>
+      </c>
+      <c r="E27" t="n">
+        <v>45</v>
+      </c>
+      <c r="F27" t="n">
+        <v>6</v>
+      </c>
+      <c r="G27" t="n">
+        <v>7</v>
+      </c>
+      <c r="H27" t="n">
+        <v>8</v>
+      </c>
+      <c r="I27" t="n">
+        <v>9</v>
+      </c>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr"/>
+      <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr"/>
+      <c r="Q27" t="inlineStr"/>
+      <c r="R27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>1</v>
+      </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="n">
+        <v>55</v>
+      </c>
+      <c r="E28" t="n">
+        <v>45</v>
+      </c>
+      <c r="F28" t="n">
+        <v>6</v>
+      </c>
+      <c r="G28" t="n">
+        <v>7</v>
+      </c>
+      <c r="H28" t="n">
+        <v>8</v>
+      </c>
+      <c r="I28" t="n">
+        <v>9</v>
+      </c>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="n">
+        <v>1</v>
+      </c>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr"/>
+      <c r="R28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>3</v>
+      </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="n">
+        <v>45</v>
+      </c>
+      <c r="E29" t="n">
+        <v>50</v>
+      </c>
+      <c r="F29" t="n">
+        <v>9</v>
+      </c>
+      <c r="G29" t="n">
+        <v>10</v>
+      </c>
+      <c r="H29" t="n">
+        <v>11</v>
+      </c>
+      <c r="I29" t="n">
+        <v>32</v>
+      </c>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr"/>
+      <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr"/>
+      <c r="R29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>1</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>33.5</v>
+      </c>
+      <c r="E30" t="n">
+        <v>33.5</v>
+      </c>
+      <c r="F30" t="n">
+        <v>90</v>
+      </c>
+      <c r="G30" t="n">
+        <v>90</v>
+      </c>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
+      <c r="N30" t="inlineStr"/>
+      <c r="O30" t="inlineStr"/>
+      <c r="P30" t="inlineStr"/>
+      <c r="Q30" t="inlineStr"/>
+      <c r="R30" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>